<commit_message>
Added some Rice varieties
added some varieties for the rice table
</commit_message>
<xml_diff>
--- a/CropDetails.xlsx
+++ b/CropDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dunura User Folders\Desktop\SDGP repo\SDGP-SE-35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511351D7-FCE4-4772-9D19-DE37DB525C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A7E61E-8E39-434F-A9FC-7030CA7EDF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F85BBFEB-AA63-49E6-BA20-671F19C6FB7C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="97">
   <si>
     <t>Plant Name</t>
   </si>
@@ -376,13 +376,228 @@
   </si>
   <si>
     <t>Finger millet</t>
+  </si>
+  <si>
+    <t>Maha season - October
+Yala season - April / May</t>
+  </si>
+  <si>
+    <t>Annual rainfall in mm. 800 – 1000 can be cultivated in any area.</t>
+  </si>
+  <si>
+    <t>Temperature between 18°C ​​– 27°C</t>
+  </si>
+  <si>
+    <t>The p.h. value between 5.0 to 8.2 is more suitable.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ravana - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Yala season (April / May). Can harvested within 100-120 days. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Oshadha - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Maha season (October). Can harvested within 100-120 days.</t>
+    </r>
+  </si>
+  <si>
+    <t>RICE VARIETIES</t>
+  </si>
+  <si>
+    <t>Pedigree </t>
+  </si>
+  <si>
+    <t>Maturity</t>
+  </si>
+  <si>
+    <t>Regions recommended for farming</t>
+  </si>
+  <si>
+    <t>Pericarp colour</t>
+  </si>
+  <si>
+    <t>Ainantsao//75-1870/Pachchaperumal</t>
+  </si>
+  <si>
+    <t>78 Days</t>
+  </si>
+  <si>
+    <t>Low Country Intermediate Zone</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Bg 367-7//IR 841/Bg 276-5</t>
+  </si>
+  <si>
+    <t>93 days</t>
+  </si>
+  <si>
+    <t>General cultivation</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Selection from At 04</t>
+  </si>
+  <si>
+    <t>88 Days</t>
+  </si>
+  <si>
+    <t>Bw 259-3 / Bw 242-5-5</t>
+  </si>
+  <si>
+    <t>90 days</t>
+  </si>
+  <si>
+    <t>Wet Zone</t>
+  </si>
+  <si>
+    <t>At 306/At 03-105</t>
+  </si>
+  <si>
+    <t>88-5089/Bg 379-2</t>
+  </si>
+  <si>
+    <t>103 – 105 days</t>
+  </si>
+  <si>
+    <t>Ld 4-9-11/Ld 99-17-4</t>
+  </si>
+  <si>
+    <t>102 days</t>
+  </si>
+  <si>
+    <t>Bg 359/Bw 267-3 (short mutant)</t>
+  </si>
+  <si>
+    <t>104 days</t>
+  </si>
+  <si>
+    <t>Wet Zone,Tolerance to iron toxicity</t>
+  </si>
+  <si>
+    <t>Bg 90-2*4/Ob 677</t>
+  </si>
+  <si>
+    <t>123 days</t>
+  </si>
+  <si>
+    <t>Major irrigation in Dry Zone &amp; Intermediate Zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bg 750</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bg 300</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ld 253</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Bw 302</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> At 311 (Neeroga)  (Basmathi type)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bg 359</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ld 368</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bw 372</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bg 380 (Hangimuththan)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bg 407H (1st Hybrid Rice)</t>
+  </si>
+  <si>
+    <t>Bg CMS 1A/IR54742-22-19-3R</t>
+  </si>
+  <si>
+    <t>118 days</t>
+  </si>
+  <si>
+    <t>High potential area</t>
+  </si>
+  <si>
+    <t>Bw 451</t>
+  </si>
+  <si>
+    <t>Bg 400-1/Bg 11-11</t>
+  </si>
+  <si>
+    <t>120 days</t>
+  </si>
+  <si>
+    <t>Low Country wet Zone</t>
+  </si>
+  <si>
+    <t>C104/Mas/Panduruwee</t>
+  </si>
+  <si>
+    <t>155 days – Maha*</t>
+  </si>
+  <si>
+    <t>Mawee land</t>
+  </si>
+  <si>
+    <t>H 9 (Photoperiod sensitive variety)</t>
+  </si>
+  <si>
+    <t>Engkatek//H 4/Podiwee A8</t>
+  </si>
+  <si>
+    <t>156 days – Maha*</t>
+  </si>
+  <si>
+    <t>Bg 38 (Photoperiod sensitive variety)</t>
+  </si>
+  <si>
+    <t>Bg 745 (Photoperiod sensitive variety)</t>
+  </si>
+  <si>
+    <t> 71-555/Podiwee A8</t>
+  </si>
+  <si>
+    <t>150 days – Maha*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,6 +624,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -418,7 +645,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -478,11 +705,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -529,8 +767,44 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -661,8 +935,8 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>6152029</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>3395382</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>7204</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -687,6 +961,50 @@
         <a:xfrm>
           <a:off x="10141322" y="6835587"/>
           <a:ext cx="6073589" cy="3361766"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>67236</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>67236</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>6039971</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>3507441</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3E17657-9B68-4277-AE69-6601B8A704AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10130118" y="19016383"/>
+          <a:ext cx="5972735" cy="3440205"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -995,15 +1313,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A40FDA2-5680-495A-A6F6-343578E817DB}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
@@ -1142,12 +1460,286 @@
       </c>
       <c r="H6" s="12"/>
     </row>
-    <row r="7" spans="1:8" ht="126" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+    <row r="7" spans="1:8" ht="291.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
         <v>35</v>
       </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:8" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Did some changes to the rice table
Did some changes to the rice table(Connected the table)
</commit_message>
<xml_diff>
--- a/CropDetails.xlsx
+++ b/CropDetails.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dunura User Folders\Desktop\SDGP repo\SDGP-SE-35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A7E61E-8E39-434F-A9FC-7030CA7EDF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9E8158-D8F4-4A4F-9D67-A794DA970CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F85BBFEB-AA63-49E6-BA20-671F19C6FB7C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F85BBFEB-AA63-49E6-BA20-671F19C6FB7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="112">
   <si>
     <t>Plant Name</t>
   </si>
@@ -253,6 +253,310 @@
 https://doa.gov.lk/rrdi_rice_varities/ </t>
   </si>
   <si>
+    <t>Finger millet</t>
+  </si>
+  <si>
+    <t>Maha season - October
+Yala season - April / May</t>
+  </si>
+  <si>
+    <t>Annual rainfall in mm. 800 – 1000 can be cultivated in any area.</t>
+  </si>
+  <si>
+    <t>Temperature between 18°C ​​– 27°C</t>
+  </si>
+  <si>
+    <t>The p.h. value between 5.0 to 8.2 is more suitable.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ravana - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Yala season (April / May). Can harvested within 100-120 days. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Oshadha - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Maha season (October). Can harvested within 100-120 days.</t>
+    </r>
+  </si>
+  <si>
+    <t>RICE VARIETIES</t>
+  </si>
+  <si>
+    <t>Pedigree </t>
+  </si>
+  <si>
+    <t>Maturity</t>
+  </si>
+  <si>
+    <t>Regions recommended for farming</t>
+  </si>
+  <si>
+    <t>Pericarp colour</t>
+  </si>
+  <si>
+    <t>Ainantsao//75-1870/Pachchaperumal</t>
+  </si>
+  <si>
+    <t>78 Days</t>
+  </si>
+  <si>
+    <t>Low Country Intermediate Zone</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Bg 367-7//IR 841/Bg 276-5</t>
+  </si>
+  <si>
+    <t>93 days</t>
+  </si>
+  <si>
+    <t>General cultivation</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Selection from At 04</t>
+  </si>
+  <si>
+    <t>88 Days</t>
+  </si>
+  <si>
+    <t>Bw 259-3 / Bw 242-5-5</t>
+  </si>
+  <si>
+    <t>90 days</t>
+  </si>
+  <si>
+    <t>Wet Zone</t>
+  </si>
+  <si>
+    <t>At 306/At 03-105</t>
+  </si>
+  <si>
+    <t>88-5089/Bg 379-2</t>
+  </si>
+  <si>
+    <t>103 – 105 days</t>
+  </si>
+  <si>
+    <t>Ld 4-9-11/Ld 99-17-4</t>
+  </si>
+  <si>
+    <t>102 days</t>
+  </si>
+  <si>
+    <t>Bg 359/Bw 267-3 (short mutant)</t>
+  </si>
+  <si>
+    <t>104 days</t>
+  </si>
+  <si>
+    <t>Wet Zone,Tolerance to iron toxicity</t>
+  </si>
+  <si>
+    <t>Bg 90-2*4/Ob 677</t>
+  </si>
+  <si>
+    <t>123 days</t>
+  </si>
+  <si>
+    <t>Major irrigation in Dry Zone &amp; Intermediate Zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bg 750</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bg 300</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ld 253</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Bw 302</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> At 311 (Neeroga)  (Basmathi type)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bg 359</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ld 368</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bw 372</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bg 380 (Hangimuththan)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bg 407H (1st Hybrid Rice)</t>
+  </si>
+  <si>
+    <t>Bg CMS 1A/IR54742-22-19-3R</t>
+  </si>
+  <si>
+    <t>118 days</t>
+  </si>
+  <si>
+    <t>High potential area</t>
+  </si>
+  <si>
+    <t>Bw 451</t>
+  </si>
+  <si>
+    <t>Bg 400-1/Bg 11-11</t>
+  </si>
+  <si>
+    <t>120 days</t>
+  </si>
+  <si>
+    <t>Low Country wet Zone</t>
+  </si>
+  <si>
+    <t>C104/Mas/Panduruwee</t>
+  </si>
+  <si>
+    <t>155 days – Maha*</t>
+  </si>
+  <si>
+    <t>Mawee land</t>
+  </si>
+  <si>
+    <t>H 9 (Photoperiod sensitive variety)</t>
+  </si>
+  <si>
+    <t>Engkatek//H 4/Podiwee A8</t>
+  </si>
+  <si>
+    <t>156 days – Maha*</t>
+  </si>
+  <si>
+    <t>Bg 38 (Photoperiod sensitive variety)</t>
+  </si>
+  <si>
+    <t>Bg 745 (Photoperiod sensitive variety)</t>
+  </si>
+  <si>
+    <t> 71-555/Podiwee A8</t>
+  </si>
+  <si>
+    <t>150 days – Maha*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum temperature is optimum (270C - 320C)
+more than 85% during Maha season
+80 % and 85 % during Yala season.
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Bg 750 - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Suitable for Low country intermediate zone. Can Harvest within 78 days.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Bg 300 - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">General cultivation. Can harvest within 93 days. </t>
+    </r>
+  </si>
+  <si>
+    <t>Ld 253 - Suitable for General cultivation. Can harvest in 88 days.</t>
+  </si>
+  <si>
+    <t>Bw 302 - Suitable for wet zone arias. Can get the harvest within 90 days.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At 311 (Neeroga Basmathi type) - General cultivation arias. Can harvest within 93 days </t>
+  </si>
+  <si>
+    <t>Bg 359 - Suitable for Wet zone. Can get the harvest within 103 - 105 days.</t>
+  </si>
+  <si>
+    <t>Ld 368 - Suitable for Wet zone Cultivation. Can get the harvest within 102 days.</t>
+  </si>
+  <si>
+    <t>Bw 372 - Sutable for Wet zone and tolerence to iorn toxicity soil. Can harvest within 104 days.</t>
+  </si>
+  <si>
+    <t>Bg 380 (Hangimuththan) - Major irrigation in dry zone and intermediate zone. Can harvest within 123 days.</t>
+  </si>
+  <si>
+    <t>Bg 407H (1st Hybrid Rice) - More sutable for High potential areas. Can harvest within 118 days.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bw 451 - Suitable for Low country wet zone. Can get the harvest within 120 days. </t>
+  </si>
+  <si>
+    <t>H 9 (Photoperiod sensitive veriety) - suitable for Mawee land. Can get the harvest within 155 days (Maha season).</t>
+  </si>
+  <si>
+    <t>Bg 38 (Photoperiod sensitive veriety) - Suitable for Mawee land. Can get the harvest within 156 days (Maha season)</t>
+  </si>
+  <si>
+    <t>Bg 745 (Photoperiod sensitive veriety) - suitable for Mawee land. Can get the harvest within 150 days (Maha season).</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -371,233 +675,295 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> can be harvested within 3 ½ months. This heirloom variety is not suitable for muddy paddy lands or any iron toxic paddy fields.  It grows well in the dry zone.
+*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bg 750 -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Suitable for Low country intermediate zone. Can Harvest within 78 days.
+*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Bg 300 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>- General cultivation. Can harvest within 93 days. 
+*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ld 253</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - Suitable for General cultivation. Can harvest in 88 days.
+*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bw 302</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - Suitable for wet zone arias. Can get the harvest within 90 days.
+*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>At 311 (Neeroga Basmathi type)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - General cultivation arias. Can harvest within 93 days.
+*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bg 359</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - Suitable for Wet zone. Can get the harvest within 103 - 105 days.
+*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ld 368</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - Suitable for Wet zone Cultivation. Can get the harvest within 102 days.
+*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bw 372</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - Sutable for Wet zone and tolerence to iorn toxicity soil. Can harvest within 104 days.
+*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bg 380</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (Hangimuththan) - Major irrigation in dry zone and intermediate zone. Can harvest within 123 days.
+*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bg 407H (1st Hybrid Rice)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - More sutable for High potential areas. Can harvest within 118 days.
+*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bw 451</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - Suitable for Low country wet zone. Can get the harvest within 120 days. 
+*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>H 9 (Photoperiod sensitive veriety)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - suitable for Mawee land. Can get the harvest within 155 days (Maha season). 
+*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Bg 38 (Photoperiod sensitive veriety) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Suitable for Mawee land. Can get the harvest within 156 days (Maha season)
+*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Bg 745 (Photoperiod sensitive veriety) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">- suitable for Mawee land. Can get the harvest within 150 days (Maha season).
 </t>
     </r>
-  </si>
-  <si>
-    <t>Finger millet</t>
-  </si>
-  <si>
-    <t>Maha season - October
-Yala season - April / May</t>
-  </si>
-  <si>
-    <t>Annual rainfall in mm. 800 – 1000 can be cultivated in any area.</t>
-  </si>
-  <si>
-    <t>Temperature between 18°C ​​– 27°C</t>
-  </si>
-  <si>
-    <t>The p.h. value between 5.0 to 8.2 is more suitable.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Ravana - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Yala season (April / May). Can harvested within 100-120 days. 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Oshadha - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Maha season (October). Can harvested within 100-120 days.</t>
-    </r>
-  </si>
-  <si>
-    <t>RICE VARIETIES</t>
-  </si>
-  <si>
-    <t>Pedigree </t>
-  </si>
-  <si>
-    <t>Maturity</t>
-  </si>
-  <si>
-    <t>Regions recommended for farming</t>
-  </si>
-  <si>
-    <t>Pericarp colour</t>
-  </si>
-  <si>
-    <t>Ainantsao//75-1870/Pachchaperumal</t>
-  </si>
-  <si>
-    <t>78 Days</t>
-  </si>
-  <si>
-    <t>Low Country Intermediate Zone</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>Bg 367-7//IR 841/Bg 276-5</t>
-  </si>
-  <si>
-    <t>93 days</t>
-  </si>
-  <si>
-    <t>General cultivation</t>
-  </si>
-  <si>
-    <t>White</t>
-  </si>
-  <si>
-    <t>Selection from At 04</t>
-  </si>
-  <si>
-    <t>88 Days</t>
-  </si>
-  <si>
-    <t>Bw 259-3 / Bw 242-5-5</t>
-  </si>
-  <si>
-    <t>90 days</t>
-  </si>
-  <si>
-    <t>Wet Zone</t>
-  </si>
-  <si>
-    <t>At 306/At 03-105</t>
-  </si>
-  <si>
-    <t>88-5089/Bg 379-2</t>
-  </si>
-  <si>
-    <t>103 – 105 days</t>
-  </si>
-  <si>
-    <t>Ld 4-9-11/Ld 99-17-4</t>
-  </si>
-  <si>
-    <t>102 days</t>
-  </si>
-  <si>
-    <t>Bg 359/Bw 267-3 (short mutant)</t>
-  </si>
-  <si>
-    <t>104 days</t>
-  </si>
-  <si>
-    <t>Wet Zone,Tolerance to iron toxicity</t>
-  </si>
-  <si>
-    <t>Bg 90-2*4/Ob 677</t>
-  </si>
-  <si>
-    <t>123 days</t>
-  </si>
-  <si>
-    <t>Major irrigation in Dry Zone &amp; Intermediate Zone</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bg 750</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bg 300</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ld 253</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Bw 302</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> At 311 (Neeroga)  (Basmathi type)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bg 359</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ld 368</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bw 372</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bg 380 (Hangimuththan)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bg 407H (1st Hybrid Rice)</t>
-  </si>
-  <si>
-    <t>Bg CMS 1A/IR54742-22-19-3R</t>
-  </si>
-  <si>
-    <t>118 days</t>
-  </si>
-  <si>
-    <t>High potential area</t>
-  </si>
-  <si>
-    <t>Bw 451</t>
-  </si>
-  <si>
-    <t>Bg 400-1/Bg 11-11</t>
-  </si>
-  <si>
-    <t>120 days</t>
-  </si>
-  <si>
-    <t>Low Country wet Zone</t>
-  </si>
-  <si>
-    <t>C104/Mas/Panduruwee</t>
-  </si>
-  <si>
-    <t>155 days – Maha*</t>
-  </si>
-  <si>
-    <t>Mawee land</t>
-  </si>
-  <si>
-    <t>H 9 (Photoperiod sensitive variety)</t>
-  </si>
-  <si>
-    <t>Engkatek//H 4/Podiwee A8</t>
-  </si>
-  <si>
-    <t>156 days – Maha*</t>
-  </si>
-  <si>
-    <t>Bg 38 (Photoperiod sensitive variety)</t>
-  </si>
-  <si>
-    <t>Bg 745 (Photoperiod sensitive variety)</t>
-  </si>
-  <si>
-    <t> 71-555/Podiwee A8</t>
-  </si>
-  <si>
-    <t>150 days – Maha*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -636,6 +1002,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -645,7 +1019,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -716,6 +1090,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -785,17 +1168,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -805,6 +1185,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1315,8 +1698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A40FDA2-5680-495A-A6F6-343578E817DB}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,7 +1710,7 @@
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="24.5703125" customWidth="1"/>
     <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="35.42578125" customWidth="1"/>
+    <col min="7" max="7" width="192.28515625" customWidth="1"/>
     <col min="8" max="8" width="93.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1389,10 +1772,12 @@
       <c r="C3" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="16" t="s">
+        <v>96</v>
+      </c>
       <c r="F3" s="2"/>
       <c r="G3" s="4" t="s">
-        <v>34</v>
+        <v>111</v>
       </c>
       <c r="H3" s="4"/>
     </row>
@@ -1462,285 +1847,328 @@
     </row>
     <row r="7" spans="1:8" ht="291.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="E7" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="F7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="17" t="s">
         <v>39</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>40</v>
       </c>
       <c r="H7" s="9"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:8" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="C12" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="D12" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="E12" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B13" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="D13" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="E13" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="21" t="s">
-        <v>49</v>
+      <c r="G13" s="21" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="D14" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="E14" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="21" t="s">
-        <v>53</v>
+      <c r="G14" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B15" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="25" t="s">
-        <v>55</v>
-      </c>
       <c r="D15" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="23" t="s">
-        <v>53</v>
+      <c r="G15" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="22" t="s">
+      <c r="B17" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" s="30" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>53</v>
+      <c r="E18" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" t="s">
+        <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="26" t="s">
+    <row r="19" spans="1:7" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="25" t="s">
-        <v>49</v>
+      <c r="G21" t="s">
+        <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>53</v>
+    <row r="22" spans="1:7" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22" t="s">
+        <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="B19" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>49</v>
+    <row r="23" spans="1:7" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" t="s">
+        <v>107</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>49</v>
+    <row r="24" spans="1:7" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="G24" t="s">
+        <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" s="23" t="s">
-        <v>53</v>
+    <row r="25" spans="1:7" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" t="s">
+        <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="B23" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="D23" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="E23" s="23" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="C24" s="22" t="s">
+    <row r="26" spans="1:7" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="D24" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="B25" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="D25" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="E25" s="23" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="D26" s="20" t="s">
-        <v>89</v>
-      </c>
       <c r="E26" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="G26" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added more data to the table
Added Rice, corn, Finger millet data to the table
</commit_message>
<xml_diff>
--- a/CropDetails.xlsx
+++ b/CropDetails.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dunura User Folders\Desktop\SDGP repo\SDGP-SE-35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9E8158-D8F4-4A4F-9D67-A794DA970CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651AA632-4C70-4B83-9C72-55245400E974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F85BBFEB-AA63-49E6-BA20-671F19C6FB7C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F85BBFEB-AA63-49E6-BA20-671F19C6FB7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="102">
   <si>
     <t>Plant Name</t>
   </si>
@@ -254,10 +254,6 @@
   </si>
   <si>
     <t>Finger millet</t>
-  </si>
-  <si>
-    <t>Maha season - October
-Yala season - April / May</t>
   </si>
   <si>
     <t>Annual rainfall in mm. 800 – 1000 can be cultivated in any area.</t>
@@ -485,86 +481,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> Bg 750 - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Suitable for Low country intermediate zone. Can Harvest within 78 days.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Bg 300 - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">General cultivation. Can harvest within 93 days. </t>
-    </r>
-  </si>
-  <si>
-    <t>Ld 253 - Suitable for General cultivation. Can harvest in 88 days.</t>
-  </si>
-  <si>
-    <t>Bw 302 - Suitable for wet zone arias. Can get the harvest within 90 days.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At 311 (Neeroga Basmathi type) - General cultivation arias. Can harvest within 93 days </t>
-  </si>
-  <si>
-    <t>Bg 359 - Suitable for Wet zone. Can get the harvest within 103 - 105 days.</t>
-  </si>
-  <si>
-    <t>Ld 368 - Suitable for Wet zone Cultivation. Can get the harvest within 102 days.</t>
-  </si>
-  <si>
-    <t>Bw 372 - Sutable for Wet zone and tolerence to iorn toxicity soil. Can harvest within 104 days.</t>
-  </si>
-  <si>
-    <t>Bg 380 (Hangimuththan) - Major irrigation in dry zone and intermediate zone. Can harvest within 123 days.</t>
-  </si>
-  <si>
-    <t>Bg 407H (1st Hybrid Rice) - More sutable for High potential areas. Can harvest within 118 days.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bw 451 - Suitable for Low country wet zone. Can get the harvest within 120 days. </t>
-  </si>
-  <si>
-    <t>H 9 (Photoperiod sensitive veriety) - suitable for Mawee land. Can get the harvest within 155 days (Maha season).</t>
-  </si>
-  <si>
-    <t>Bg 38 (Photoperiod sensitive veriety) - Suitable for Mawee land. Can get the harvest within 156 days (Maha season)</t>
-  </si>
-  <si>
-    <t>Bg 745 (Photoperiod sensitive veriety) - suitable for Mawee land. Can get the harvest within 150 days (Maha season).</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>* Suwadel -</t>
     </r>
     <r>
@@ -957,13 +873,149 @@
       <t xml:space="preserve">- suitable for Mawee land. Can get the harvest within 150 days (Maha season).
 </t>
     </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Source -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> https://doa.gov.lk/crop-production</t>
+    </r>
+  </si>
+  <si>
+    <t>A deep sandy loam soil with good drainage is ideal.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">K A 02 - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Suitable for Dry zone. More suited to growing in the Yala season. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Arunalu - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Suitable for Yala season. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">MI HOT - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Suitable for Dry and Wet zones. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">MI GREEN - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">More suitable for the Northern Province.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Southern dry zone</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Maha season - October
+Yala season - April / May
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Sourse -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> https://doa.gov.lk/fcrdi-rardckilinochchi-crops/</t>
+    </r>
+  </si>
+  <si>
+    <t>600 mm in the arid areas to 6,000 mm in the very wet areas.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -998,14 +1050,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1186,7 +1230,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1388,6 +1432,50 @@
         <a:xfrm>
           <a:off x="10130118" y="19016383"/>
           <a:ext cx="5972735" cy="3440205"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>67234</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>112058</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>6196851</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>3171263</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEE4FAC8-6E8B-13AF-E768-895ED0054C19}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20876558" y="8236323"/>
+          <a:ext cx="6129617" cy="3059205"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1698,8 +1786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A40FDA2-5680-495A-A6F6-343578E817DB}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1710,7 +1798,7 @@
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="24.5703125" customWidth="1"/>
     <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="192.28515625" customWidth="1"/>
+    <col min="7" max="7" width="167.7109375" customWidth="1"/>
     <col min="8" max="8" width="93.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1772,16 +1860,19 @@
       <c r="C3" s="17" t="s">
         <v>33</v>
       </c>
+      <c r="D3" s="16" t="s">
+        <v>101</v>
+      </c>
       <c r="E3" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="4" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8" ht="175.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="309.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>16</v>
       </c>
@@ -1797,8 +1888,12 @@
       <c r="E4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="4"/>
+      <c r="F4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:8" ht="267" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1849,320 +1944,282 @@
       <c r="A7" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="9"/>
+      <c r="B7" s="16" t="s">
+        <v>99</v>
+      </c>
       <c r="C7" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="E7" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="F7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="17" t="s">
         <v>38</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>39</v>
       </c>
       <c r="H7" s="9"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:8" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="C12" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="D12" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="E12" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B13" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="D13" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="E13" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>97</v>
-      </c>
+      <c r="G13" s="21"/>
     </row>
     <row r="14" spans="1:8" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B14" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="D14" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="E14" s="21" t="s">
         <v>51</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="G14" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="25" t="s">
-        <v>54</v>
-      </c>
       <c r="D15" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="23" t="s">
         <v>51</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="G15" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B16" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="D16" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>57</v>
-      </c>
       <c r="E16" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" t="s">
-        <v>100</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="26" t="s">
-        <v>51</v>
-      </c>
       <c r="E17" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="G17" s="30" t="s">
-        <v>101</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="G17" s="30"/>
     </row>
     <row r="18" spans="1:7" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B18" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="22" t="s">
-        <v>60</v>
-      </c>
       <c r="D18" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="G18" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B19" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="25" t="s">
-        <v>62</v>
-      </c>
       <c r="D19" s="26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="G19" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B20" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="D20" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="20" t="s">
-        <v>65</v>
-      </c>
       <c r="E20" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="G20" t="s">
-        <v>104</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B21" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="D21" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="D21" s="24" t="s">
-        <v>68</v>
-      </c>
       <c r="E21" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="G21" t="s">
-        <v>105</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="C22" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="D22" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="D22" s="19" t="s">
-        <v>81</v>
-      </c>
       <c r="E22" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="G22" t="s">
-        <v>106</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="C23" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="D23" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="D23" s="24" t="s">
-        <v>85</v>
-      </c>
       <c r="E23" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="G23" t="s">
-        <v>107</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B24" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="D24" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="D24" s="20" t="s">
-        <v>88</v>
-      </c>
       <c r="E24" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="G24" t="s">
-        <v>108</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B25" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="C25" s="25" t="s">
-        <v>91</v>
-      </c>
       <c r="D25" s="24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="G25" t="s">
-        <v>109</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="C26" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="22" t="s">
-        <v>95</v>
-      </c>
       <c r="D26" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="G26" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added more details for the CropDetails table
added places and some more data to the table.
</commit_message>
<xml_diff>
--- a/CropDetails.xlsx
+++ b/CropDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dunura User Folders\Desktop\SDGP repo\SDGP-SE-35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651AA632-4C70-4B83-9C72-55245400E974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{563CD7B5-008A-4BF4-8FBC-33C7FFC1C7F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F85BBFEB-AA63-49E6-BA20-671F19C6FB7C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="103">
   <si>
     <t>Plant Name</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>May to August. Yala Kanna is the main growing season of onions, bulbs are grown as Yala Kanna and Maha Kanna for seeds.</t>
-  </si>
-  <si>
-    <t>Mainly in dry zone. Can be cultivated in areas from sea level to 2000 meters.</t>
   </si>
   <si>
     <t>Maximum raifall during the cultivation period should not exceed 750mm.</t>
@@ -156,9 +153,6 @@
     <t>Chilli</t>
   </si>
   <si>
-    <t>Chilli can be grown from sea level to about 1600 meters high.</t>
-  </si>
-  <si>
     <t>Annual rainfall in  600 – 1000 mm. can be cultivated in existing areas.</t>
   </si>
   <si>
@@ -229,19 +223,11 @@
     <t>The p.h. value between 5.8 to 7.0 is more suitable.</t>
   </si>
   <si>
-    <t>Dry and temperate zones are best suited for commercial cultivation.</t>
-  </si>
-  <si>
     <t>The maximum annual rainfall is about 600 -1000 mm.</t>
   </si>
   <si>
     <t>The temperature required for successful growth is 25 – 30 °C.
 The corn plant needs full sun.</t>
-  </si>
-  <si>
-    <t>Badhra - Harvest time is between 105-110 days.
-M.I.Mase Hybrid 01 &amp; M.I.Mase Hybrid  - Harvest time is between 105-110 days.
-M.I.Mase Hybrid 03 - Harvest time is between 100-105 days.</t>
   </si>
   <si>
     <t>Mainly in Maha season.  
@@ -898,91 +884,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">K A 02 - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Suitable for Dry zone. More suited to growing in the Yala season. 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Arunalu - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Suitable for Yala season. 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">MI HOT - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Suitable for Dry and Wet zones. 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">MI GREEN - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">More suitable for the Northern Province.
-</t>
-    </r>
-  </si>
-  <si>
-    <t>Southern dry zone</t>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Maha season - October
 Yala season - April / May
 </t>
@@ -1009,6 +910,173 @@
   </si>
   <si>
     <t>600 mm in the arid areas to 6,000 mm in the very wet areas.</t>
+  </si>
+  <si>
+    <t>Mainly in dry zone. Can be cultivated in areas from sea level to 2000 meters.
+Matale and Anuradhapura,
+Galewela, Dambulla, Kimbissa, Maradankadawala,
+Polonnaruwa, Kurunagala, Vavuniya, Mullaitive,
+Mannar</t>
+  </si>
+  <si>
+    <t>Anuradhapura, Kurunagala, Ampara, Polonnaruwa, Batticaloa, Hambanthota, Monaragala, Trincomalee, Kilinochchi, Badulla, Vavuniya, Mannar, Matale, Mulativu, Puttalam, Ratnapura, Kandy, Matara, Gampaha, Jaffna, Kalutara, Galle, Kegalle, Colombo, NuwaraEliya</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Badhra </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">- Harvest time is between 105-110 days.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>M.I.Mase Hybrid 01 &amp; M.I.Mase Hybrid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  - Harvest time is between 105-110 days.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>M.I.Mase Hybrid 03</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - Harvest time is between 100-105 days.</t>
+    </r>
+  </si>
+  <si>
+    <t>Chilli can be grown from sea level to about 1600 meters high.
+Anuradhapura, Polonnaruwa,
+Kurunagala,
+Matale, Puttalam</t>
+  </si>
+  <si>
+    <t>Dry and temperate zones are best suited for commercial cultivation.
+Ampara, Anuradhapura, Polonnaruwa, Kurunagala, Moneragala, Badulla, Matale</t>
+  </si>
+  <si>
+    <t>Southern dry zone
+Kurunagala, Anuradhapura, Moneragala, Polonnaruwa, Badulla, Matale</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">K A 02 - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Suitable for Dry zone. More suited to growing in the Yala season. Can harvest in 60 to 90 days.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Arunalu - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Suitable for Yala season. Can harvest in 60 to 70 days.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">MI HOT - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Suitable for Dry and Wet zones. 60 to 70 days for harvest.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">MI GREEN - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">More suitable for the Northern Province. 60 to 70 days 
+</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1786,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A40FDA2-5680-495A-A6F6-343578E817DB}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1828,398 +1896,402 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="207.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="254.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>96</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" ht="409.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="C3" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="F3" s="2"/>
+        <v>91</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="G3" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" ht="309.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="E4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:8" ht="267" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>32</v>
-      </c>
       <c r="D5" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>31</v>
+        <v>98</v>
       </c>
       <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" ht="409.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="12"/>
       <c r="E6" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H6" s="12"/>
     </row>
     <row r="7" spans="1:8" ht="291.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="17" t="s">
         <v>34</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>38</v>
       </c>
       <c r="H7" s="9"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:8" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G13" s="21"/>
     </row>
     <row r="14" spans="1:8" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="23" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="27" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G17" s="30"/>
     </row>
     <row r="18" spans="1:7" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="27" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="28" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="29" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>